<commit_message>
Add mode selection & Range sResult in xlsx
</commit_message>
<xml_diff>
--- a/Code/Result/Result.xlsx
+++ b/Code/Result/Result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://upsud-my.sharepoint.com/personal/jiahua_tang_universite-paris-saclay_fr/Documents/Julia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emnormandie1-my.sharepoint.com/personal/jtang_em-normandie_fr/Documents/2EVRPMM/Code/Result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="488" documentId="8_{92A22CC0-19AB-D84A-B77D-FA4F4CDBC343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3E57A33-7798-534C-95B9-57FB1FCA1456}"/>
+  <xr:revisionPtr revIDLastSave="560" documentId="8_{92A22CC0-19AB-D84A-B77D-FA4F4CDBC343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9BF7E1C-66A4-4ADF-8C5E-5F2D0D4CE296}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19880" activeTab="2" xr2:uid="{8802EF90-BEE6-8145-AE6F-1EA5C18B901E}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{8802EF90-BEE6-8145-AE6F-1EA5C18B901E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="95">
   <si>
     <t>      Model Name: Mac mini</t>
   </si>
@@ -250,9 +250,6 @@
     <t>Log</t>
   </si>
   <si>
-    <t>Execution Time</t>
-  </si>
-  <si>
     <t>Total distance</t>
   </si>
   <si>
@@ -332,24 +329,40 @@
   </si>
   <si>
     <t>Speed SEV</t>
+  </si>
+  <si>
+    <t>Execution Time (sec)</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Optimal / 120min</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Optimal / 140min</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Feasible / 140min</t>
+    <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -364,14 +377,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="4"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="等线"/>
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -568,7 +581,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -665,9 +678,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -682,12 +701,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1009,22 +1024,22 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.36328125" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
-    <col min="5" max="5" width="15.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.6328125" customWidth="1"/>
+    <col min="6" max="6" width="13.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6">
       <c r="A1" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
         <v>20</v>
       </c>
@@ -1034,7 +1049,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
@@ -1042,7 +1057,7 @@
       <c r="E3" s="3"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="4">
@@ -1058,7 +1073,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -1076,7 +1091,7 @@
       </c>
       <c r="F5" s="7"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -1091,7 +1106,7 @@
       </c>
       <c r="F6" s="7"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6">
       <c r="B7" s="1">
         <v>6</v>
       </c>
@@ -1106,7 +1121,7 @@
       </c>
       <c r="F7" s="7"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="B8" s="1">
         <v>8</v>
       </c>
@@ -1123,7 +1138,7 @@
         <v>849.53</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6">
       <c r="A9" s="3"/>
       <c r="B9" s="4">
         <v>10</v>
@@ -1139,67 +1154,67 @@
       </c>
       <c r="F9" s="8"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6">
       <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6">
       <c r="A15" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6">
       <c r="A16" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1">
       <c r="A17" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1">
       <c r="A18" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1">
       <c r="A19" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1">
       <c r="A20" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1">
       <c r="A21" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1">
       <c r="A23" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1">
       <c r="A24" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1">
       <c r="A25" s="2" t="s">
         <v>11</v>
       </c>
@@ -1219,13 +1234,13 @@
       <selection activeCell="B1" sqref="B1:G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="14.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.83203125" customWidth="1"/>
+    <col min="2" max="2" width="14.36328125" customWidth="1"/>
+    <col min="3" max="3" width="13.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="1" customFormat="1">
       <c r="B1" s="1" t="s">
         <v>33</v>
       </c>
@@ -1242,7 +1257,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>30</v>
       </c>
@@ -1256,7 +1271,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1270,7 +1285,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>35</v>
       </c>
@@ -1284,7 +1299,7 @@
         <v>835</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1299,39 +1314,43 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2688DEF4-29AA-4D4A-9F28-57B6F8D7E4AE}">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P1" sqref="O1:P1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="88" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" customWidth="1"/>
-    <col min="3" max="4" width="11.6640625" customWidth="1"/>
-    <col min="5" max="5" width="9.5" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" customWidth="1"/>
-    <col min="8" max="9" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="13.81640625" hidden="1" customWidth="1"/>
+    <col min="3" max="4" width="11.6328125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="8.81640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" hidden="1" customWidth="1"/>
+    <col min="8" max="9" width="9.453125" hidden="1" customWidth="1"/>
+    <col min="10" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6328125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="12.453125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.26953125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.26953125" customWidth="1"/>
+    <col min="16" max="16" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18">
       <c r="A3" s="17"/>
       <c r="B3" s="18" t="s">
         <v>33</v>
@@ -1352,10 +1371,10 @@
         <v>60</v>
       </c>
       <c r="H3" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="I3" s="28" t="s">
         <v>90</v>
-      </c>
-      <c r="I3" s="28" t="s">
-        <v>91</v>
       </c>
       <c r="J3" s="28" t="s">
         <v>61</v>
@@ -1367,22 +1386,23 @@
         <v>62</v>
       </c>
       <c r="M3" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="N3" s="19" t="s">
+        <v>91</v>
+      </c>
+      <c r="O3" s="19"/>
+      <c r="P3" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="N3" s="19" t="s">
-        <v>64</v>
-      </c>
-      <c r="O3" s="19" t="s">
+      <c r="Q3" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="P3" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="Q3" s="20" t="s">
+      <c r="R3" s="20" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18">
       <c r="A4" s="23" t="s">
         <v>43</v>
       </c>
@@ -1399,29 +1419,31 @@
         <v>10000</v>
       </c>
       <c r="F4" s="25">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G4" s="25">
-        <v>100</v>
-      </c>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
+        <v>50</v>
+      </c>
+      <c r="H4" s="25">
+        <v>1</v>
+      </c>
+      <c r="I4" s="25">
+        <v>1</v>
+      </c>
       <c r="J4" s="25">
         <v>25</v>
       </c>
       <c r="K4" s="25">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L4" s="26">
         <v>10</v>
       </c>
-      <c r="M4" s="27"/>
-      <c r="N4" s="25"/>
-      <c r="O4" s="25"/>
       <c r="P4" s="25"/>
-      <c r="Q4" s="26"/>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q4" s="25"/>
+      <c r="R4" s="26"/>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" s="15" t="s">
         <v>44</v>
       </c>
@@ -1438,24 +1460,30 @@
         <v>10000</v>
       </c>
       <c r="F5">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G5">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H5">
+        <v>1</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
       </c>
       <c r="J5">
         <v>25</v>
       </c>
       <c r="K5">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L5" s="12">
         <v>10</v>
       </c>
       <c r="M5" s="11"/>
-      <c r="Q5" s="12"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R5" s="12"/>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6" s="15" t="s">
         <v>45</v>
       </c>
@@ -1472,24 +1500,30 @@
         <v>10000</v>
       </c>
       <c r="F6">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G6">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
       </c>
       <c r="J6">
         <v>25</v>
       </c>
       <c r="K6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L6" s="12">
         <v>10</v>
       </c>
       <c r="M6" s="11"/>
-      <c r="Q6" s="12"/>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R6" s="12"/>
+    </row>
+    <row r="7" spans="1:18">
       <c r="A7" s="15" t="s">
         <v>46</v>
       </c>
@@ -1506,24 +1540,30 @@
         <v>10000</v>
       </c>
       <c r="F7">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G7">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
       </c>
       <c r="J7">
         <v>25</v>
       </c>
       <c r="K7">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L7" s="12">
         <v>10</v>
       </c>
       <c r="M7" s="11"/>
-      <c r="Q7" s="12"/>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R7" s="12"/>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8" s="16" t="s">
         <v>47</v>
       </c>
@@ -1540,18 +1580,22 @@
         <v>10000</v>
       </c>
       <c r="F8" s="3">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G8" s="3">
-        <v>100</v>
-      </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="H8" s="3">
+        <v>1</v>
+      </c>
+      <c r="I8" s="3">
+        <v>1</v>
+      </c>
       <c r="J8" s="3">
         <v>25</v>
       </c>
       <c r="K8" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L8" s="14">
         <v>10</v>
@@ -1560,9 +1604,10 @@
       <c r="N8" s="3"/>
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
-      <c r="Q8" s="14"/>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q8" s="3"/>
+      <c r="R8" s="14"/>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9" s="15" t="s">
         <v>48</v>
       </c>
@@ -1579,24 +1624,30 @@
         <v>10000</v>
       </c>
       <c r="F9">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G9">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H9" s="25">
+        <v>1</v>
+      </c>
+      <c r="I9" s="25">
+        <v>1</v>
       </c>
       <c r="J9">
         <v>25</v>
       </c>
       <c r="K9">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L9" s="12">
         <v>10</v>
       </c>
       <c r="M9" s="11"/>
-      <c r="Q9" s="12"/>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R9" s="12"/>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10" s="15" t="s">
         <v>49</v>
       </c>
@@ -1613,24 +1664,30 @@
         <v>10000</v>
       </c>
       <c r="F10">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G10">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
       </c>
       <c r="J10">
         <v>25</v>
       </c>
       <c r="K10">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L10" s="12">
         <v>10</v>
       </c>
       <c r="M10" s="11"/>
-      <c r="Q10" s="12"/>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R10" s="12"/>
+    </row>
+    <row r="11" spans="1:18">
       <c r="A11" s="15" t="s">
         <v>50</v>
       </c>
@@ -1647,24 +1704,30 @@
         <v>10000</v>
       </c>
       <c r="F11">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G11">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
       </c>
       <c r="J11">
         <v>25</v>
       </c>
       <c r="K11">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L11" s="12">
         <v>10</v>
       </c>
       <c r="M11" s="11"/>
-      <c r="Q11" s="12"/>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R11" s="12"/>
+    </row>
+    <row r="12" spans="1:18">
       <c r="A12" s="15" t="s">
         <v>51</v>
       </c>
@@ -1681,24 +1744,30 @@
         <v>10000</v>
       </c>
       <c r="F12">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G12">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
       </c>
       <c r="J12">
         <v>25</v>
       </c>
       <c r="K12">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L12" s="12">
         <v>10</v>
       </c>
       <c r="M12" s="11"/>
-      <c r="Q12" s="12"/>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R12" s="12"/>
+    </row>
+    <row r="13" spans="1:18">
       <c r="A13" s="15" t="s">
         <v>52</v>
       </c>
@@ -1715,18 +1784,22 @@
         <v>10000</v>
       </c>
       <c r="F13" s="3">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G13" s="3">
-        <v>100</v>
-      </c>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="H13" s="3">
+        <v>1</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
       <c r="J13" s="3">
         <v>25</v>
       </c>
       <c r="K13" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L13" s="14">
         <v>10</v>
@@ -1735,14 +1808,15 @@
       <c r="N13" s="3"/>
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
-      <c r="Q13" s="14"/>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q13" s="3"/>
+      <c r="R13" s="14"/>
+    </row>
+    <row r="14" spans="1:18">
       <c r="A14" s="27" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C14" s="25">
         <v>19.36</v>
@@ -1754,18 +1828,22 @@
         <v>10000</v>
       </c>
       <c r="F14" s="25">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G14" s="25">
-        <v>100</v>
-      </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
+        <v>50</v>
+      </c>
+      <c r="H14" s="25">
+        <v>1</v>
+      </c>
+      <c r="I14" s="25">
+        <v>1</v>
+      </c>
       <c r="J14" s="25">
         <v>25</v>
       </c>
       <c r="K14" s="25">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L14" s="26">
         <v>10</v>
@@ -1774,14 +1852,15 @@
       <c r="N14" s="25"/>
       <c r="O14" s="25"/>
       <c r="P14" s="25"/>
-      <c r="Q14" s="26"/>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q14" s="25"/>
+      <c r="R14" s="26"/>
+    </row>
+    <row r="15" spans="1:18">
       <c r="A15" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C15">
         <v>19.36</v>
@@ -1793,29 +1872,35 @@
         <v>10000</v>
       </c>
       <c r="F15">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G15">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>1</v>
       </c>
       <c r="J15">
         <v>25</v>
       </c>
       <c r="K15">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L15" s="12">
         <v>10</v>
       </c>
       <c r="M15" s="11"/>
-      <c r="Q15" s="12"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R15" s="12"/>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C16">
         <v>19.36</v>
@@ -1827,29 +1912,35 @@
         <v>10000</v>
       </c>
       <c r="F16">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G16">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
       </c>
       <c r="J16">
         <v>25</v>
       </c>
       <c r="K16">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L16" s="12">
         <v>10</v>
       </c>
       <c r="M16" s="11"/>
-      <c r="Q16" s="12"/>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R16" s="12"/>
+    </row>
+    <row r="17" spans="1:18">
       <c r="A17" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C17">
         <v>19.36</v>
@@ -1861,29 +1952,35 @@
         <v>10000</v>
       </c>
       <c r="F17">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G17">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
       </c>
       <c r="J17">
         <v>25</v>
       </c>
       <c r="K17">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L17" s="12">
         <v>10</v>
       </c>
       <c r="M17" s="11"/>
-      <c r="Q17" s="12"/>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R17" s="12"/>
+    </row>
+    <row r="18" spans="1:18">
       <c r="A18" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B18" s="22" t="s">
         <v>72</v>
-      </c>
-      <c r="B18" s="22" t="s">
-        <v>73</v>
       </c>
       <c r="C18" s="3">
         <v>19.36</v>
@@ -1895,18 +1992,22 @@
         <v>10000</v>
       </c>
       <c r="F18" s="3">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G18" s="3">
-        <v>100</v>
-      </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="H18" s="3">
+        <v>1</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1</v>
+      </c>
       <c r="J18" s="3">
         <v>25</v>
       </c>
       <c r="K18" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="L18" s="14">
         <v>10</v>
@@ -1915,11 +2016,12 @@
       <c r="N18" s="3"/>
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
-      <c r="Q18" s="14"/>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q18" s="3"/>
+      <c r="R18" s="14"/>
+    </row>
+    <row r="19" spans="1:18">
       <c r="A19" s="23" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B19" s="24" t="s">
         <v>53</v>
@@ -1928,19 +2030,19 @@
         <v>16.47</v>
       </c>
       <c r="D19" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E19" s="27">
         <v>10000</v>
       </c>
       <c r="F19" s="25">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G19" s="25">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="H19" s="25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I19" s="25">
         <v>1</v>
@@ -1954,15 +2056,20 @@
       <c r="L19" s="26">
         <v>10</v>
       </c>
-      <c r="M19" s="27"/>
-      <c r="N19" s="25"/>
+      <c r="M19" s="27">
+        <v>1094.49</v>
+      </c>
+      <c r="N19" s="25">
+        <v>985.05200000000002</v>
+      </c>
       <c r="O19" s="25"/>
       <c r="P19" s="25"/>
-      <c r="Q19" s="26"/>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q19" s="25"/>
+      <c r="R19" s="26"/>
+    </row>
+    <row r="20" spans="1:18">
       <c r="A20" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B20" s="21" t="s">
         <v>53</v>
@@ -1971,16 +2078,22 @@
         <v>16.47</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E20" s="11">
         <v>10000</v>
       </c>
       <c r="F20">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G20">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
       </c>
       <c r="J20">
         <v>16</v>
@@ -1991,12 +2104,20 @@
       <c r="L20" s="12">
         <v>10</v>
       </c>
-      <c r="M20" s="11"/>
-      <c r="Q20" s="12"/>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M20" s="11">
+        <v>1094.26</v>
+      </c>
+      <c r="N20" s="33">
+        <v>1455.43</v>
+      </c>
+      <c r="O20" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="R20" s="12"/>
+    </row>
+    <row r="21" spans="1:18">
       <c r="A21" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B21" s="21" t="s">
         <v>53</v>
@@ -2005,16 +2126,22 @@
         <v>16.47</v>
       </c>
       <c r="D21" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E21" s="11">
         <v>10000</v>
       </c>
       <c r="F21">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G21">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
       </c>
       <c r="J21">
         <v>16</v>
@@ -2025,12 +2152,20 @@
       <c r="L21" s="12">
         <v>10</v>
       </c>
-      <c r="M21" s="11"/>
-      <c r="Q21" s="12"/>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M21" s="33">
+        <v>1094.49</v>
+      </c>
+      <c r="N21" s="33">
+        <v>2801.37</v>
+      </c>
+      <c r="O21" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="R21" s="12"/>
+    </row>
+    <row r="22" spans="1:18">
       <c r="A22" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B22" s="21" t="s">
         <v>53</v>
@@ -2039,16 +2174,22 @@
         <v>16.47</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E22" s="11">
         <v>10000</v>
       </c>
       <c r="F22">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G22">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
       </c>
       <c r="J22">
         <v>16</v>
@@ -2059,12 +2200,20 @@
       <c r="L22" s="12">
         <v>10</v>
       </c>
-      <c r="M22" s="11"/>
-      <c r="Q22" s="12"/>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M22" s="11">
+        <v>1092.27</v>
+      </c>
+      <c r="N22" s="33">
+        <v>4577.79</v>
+      </c>
+      <c r="O22" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="R22" s="12"/>
+    </row>
+    <row r="23" spans="1:18">
       <c r="A23" s="16" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B23" s="22" t="s">
         <v>53</v>
@@ -2073,19 +2222,23 @@
         <v>16.47</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E23" s="13">
         <v>10000</v>
       </c>
       <c r="F23" s="3">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G23" s="3">
-        <v>100</v>
-      </c>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="H23" s="3">
+        <v>1</v>
+      </c>
+      <c r="I23" s="3">
+        <v>1</v>
+      </c>
       <c r="J23" s="3">
         <v>16</v>
       </c>
@@ -2095,15 +2248,20 @@
       <c r="L23" s="14">
         <v>10</v>
       </c>
-      <c r="M23" s="13"/>
-      <c r="N23" s="3"/>
+      <c r="M23" s="11">
+        <v>860.03</v>
+      </c>
+      <c r="N23" s="3">
+        <v>800.68499999999995</v>
+      </c>
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
-      <c r="Q23" s="14"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q23" s="3"/>
+      <c r="R23" s="14"/>
+    </row>
+    <row r="24" spans="1:18">
       <c r="A24" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B24" s="21" t="s">
         <v>54</v>
@@ -2112,16 +2270,22 @@
         <v>16.47</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E24" s="11">
         <v>10000</v>
       </c>
       <c r="F24">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G24">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H24" s="25">
+        <v>1</v>
+      </c>
+      <c r="I24" s="25">
+        <v>1</v>
       </c>
       <c r="J24">
         <v>16</v>
@@ -2129,15 +2293,23 @@
       <c r="K24">
         <v>10</v>
       </c>
-      <c r="L24" s="12">
-        <v>10</v>
-      </c>
-      <c r="M24" s="11"/>
-      <c r="Q24" s="12"/>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="L24" s="32">
+        <v>10</v>
+      </c>
+      <c r="M24" s="27">
+        <v>979.4</v>
+      </c>
+      <c r="N24" s="33">
+        <v>513.24800000000005</v>
+      </c>
+      <c r="O24" s="33" t="s">
+        <v>93</v>
+      </c>
+      <c r="R24" s="12"/>
+    </row>
+    <row r="25" spans="1:18">
       <c r="A25" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B25" s="21" t="s">
         <v>54</v>
@@ -2146,16 +2318,22 @@
         <v>16.47</v>
       </c>
       <c r="D25" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E25" s="11">
         <v>10000</v>
       </c>
       <c r="F25">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G25">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
       </c>
       <c r="J25">
         <v>16</v>
@@ -2166,12 +2344,20 @@
       <c r="L25" s="12">
         <v>10</v>
       </c>
-      <c r="M25" s="11"/>
-      <c r="Q25" s="12"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M25" s="11">
+        <v>963.58</v>
+      </c>
+      <c r="N25" s="33">
+        <v>8412.07</v>
+      </c>
+      <c r="O25" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="R25" s="12"/>
+    </row>
+    <row r="26" spans="1:18">
       <c r="A26" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B26" s="21" t="s">
         <v>54</v>
@@ -2180,16 +2366,22 @@
         <v>16.47</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E26" s="11">
         <v>10000</v>
       </c>
       <c r="F26">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G26">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
       </c>
       <c r="J26">
         <v>16</v>
@@ -2201,11 +2393,11 @@
         <v>10</v>
       </c>
       <c r="M26" s="11"/>
-      <c r="Q26" s="12"/>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R26" s="12"/>
+    </row>
+    <row r="27" spans="1:18">
       <c r="A27" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B27" s="21" t="s">
         <v>54</v>
@@ -2214,16 +2406,22 @@
         <v>16.47</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E27" s="11">
         <v>10000</v>
       </c>
       <c r="F27">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G27">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
       </c>
       <c r="J27">
         <v>16</v>
@@ -2234,12 +2432,20 @@
       <c r="L27" s="12">
         <v>10</v>
       </c>
-      <c r="M27" s="11"/>
-      <c r="Q27" s="12"/>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="M27" s="11">
+        <v>874.51</v>
+      </c>
+      <c r="N27" s="33">
+        <v>8412.59</v>
+      </c>
+      <c r="O27" s="33" t="s">
+        <v>94</v>
+      </c>
+      <c r="R27" s="12"/>
+    </row>
+    <row r="28" spans="1:18">
       <c r="A28" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B28" s="22" t="s">
         <v>54</v>
@@ -2248,19 +2454,23 @@
         <v>16.47</v>
       </c>
       <c r="D28" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E28" s="13">
         <v>10000</v>
       </c>
       <c r="F28" s="3">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G28" s="3">
-        <v>100</v>
-      </c>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="H28" s="3">
+        <v>1</v>
+      </c>
+      <c r="I28" s="3">
+        <v>1</v>
+      </c>
       <c r="J28" s="3">
         <v>16</v>
       </c>
@@ -2270,36 +2480,47 @@
       <c r="L28" s="14">
         <v>10</v>
       </c>
-      <c r="M28" s="13"/>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
+      <c r="M28" s="13">
+        <v>942.03</v>
+      </c>
+      <c r="N28" s="3">
+        <v>2470.12</v>
+      </c>
+      <c r="O28" s="33" t="s">
+        <v>93</v>
+      </c>
       <c r="P28" s="3"/>
-      <c r="Q28" s="14"/>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q28" s="3"/>
+      <c r="R28" s="14"/>
+    </row>
+    <row r="29" spans="1:18">
       <c r="A29" s="27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B29" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C29" s="25">
         <v>16.47</v>
       </c>
       <c r="D29" s="29" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E29" s="27">
         <v>10000</v>
       </c>
       <c r="F29" s="25">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G29" s="25">
-        <v>100</v>
-      </c>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
+        <v>50</v>
+      </c>
+      <c r="H29" s="25">
+        <v>1</v>
+      </c>
+      <c r="I29" s="25">
+        <v>1</v>
+      </c>
       <c r="J29" s="25">
         <v>16</v>
       </c>
@@ -2313,29 +2534,36 @@
       <c r="N29" s="25"/>
       <c r="O29" s="25"/>
       <c r="P29" s="25"/>
-      <c r="Q29" s="26"/>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="Q29" s="25"/>
+      <c r="R29" s="26"/>
+    </row>
+    <row r="30" spans="1:18">
       <c r="A30" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B30" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C30">
         <v>16.47</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E30" s="11">
         <v>10000</v>
       </c>
       <c r="F30">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G30">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>1</v>
       </c>
       <c r="J30">
         <v>16</v>
@@ -2347,29 +2575,35 @@
         <v>10</v>
       </c>
       <c r="M30" s="11"/>
-      <c r="Q30" s="12"/>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R30" s="12"/>
+    </row>
+    <row r="31" spans="1:18">
       <c r="A31" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C31">
         <v>16.47</v>
       </c>
       <c r="D31" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E31" s="11">
         <v>10000</v>
       </c>
       <c r="F31">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G31">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>1</v>
       </c>
       <c r="J31">
         <v>16</v>
@@ -2381,29 +2615,35 @@
         <v>10</v>
       </c>
       <c r="M31" s="11"/>
-      <c r="Q31" s="12"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R31" s="12"/>
+    </row>
+    <row r="32" spans="1:18">
       <c r="A32" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B32" s="21" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C32">
         <v>16.47</v>
       </c>
       <c r="D32" s="30" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E32" s="11">
         <v>10000</v>
       </c>
       <c r="F32">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G32">
-        <v>100</v>
+        <v>50</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>1</v>
       </c>
       <c r="J32">
         <v>16</v>
@@ -2415,32 +2655,36 @@
         <v>10</v>
       </c>
       <c r="M32" s="11"/>
-      <c r="Q32" s="12"/>
-    </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="R32" s="12"/>
+    </row>
+    <row r="33" spans="1:18">
       <c r="A33" s="13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B33" s="22" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C33" s="3">
         <v>16.47</v>
       </c>
       <c r="D33" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E33" s="13">
         <v>10000</v>
       </c>
       <c r="F33" s="3">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="G33" s="3">
-        <v>100</v>
-      </c>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="H33" s="3">
+        <v>1</v>
+      </c>
+      <c r="I33" s="3">
+        <v>1</v>
+      </c>
       <c r="J33" s="3">
         <v>16</v>
       </c>
@@ -2454,7 +2698,8 @@
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
-      <c r="Q33" s="14"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="14"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Add compare code of 10/16 parkings
</commit_message>
<xml_diff>
--- a/Code/Result/Result.xlsx
+++ b/Code/Result/Result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emnormandie1-my.sharepoint.com/personal/jtang_em-normandie_fr/Documents/2EVRPMM/Code/Result/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="560" documentId="8_{92A22CC0-19AB-D84A-B77D-FA4F4CDBC343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9BF7E1C-66A4-4ADF-8C5E-5F2D0D4CE296}"/>
+  <xr:revisionPtr revIDLastSave="587" documentId="8_{92A22CC0-19AB-D84A-B77D-FA4F4CDBC343}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6FD882E5-44B1-4D3D-8494-349010E7C7E3}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" activeTab="2" xr2:uid="{8802EF90-BEE6-8145-AE6F-1EA5C18B901E}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{8802EF90-BEE6-8145-AE6F-1EA5C18B901E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="98">
   <si>
     <t>      Model Name: Mac mini</t>
   </si>
@@ -344,6 +344,18 @@
   </si>
   <si>
     <t>Feasible / 140min</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Total distance </t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fixed</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>Random</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -678,10 +690,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -699,6 +711,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1321,36 +1337,49 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2688DEF4-29AA-4D4A-9F28-57B6F8D7E4AE}">
-  <dimension ref="A1:R33"/>
+  <dimension ref="A1:T33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="88" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="13.81640625" hidden="1" customWidth="1"/>
-    <col min="3" max="4" width="11.6328125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="9.453125" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="8.81640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="9.1796875" hidden="1" customWidth="1"/>
-    <col min="8" max="9" width="9.453125" hidden="1" customWidth="1"/>
-    <col min="10" max="11" width="0" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="12.6328125" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.6328125" customWidth="1"/>
     <col min="13" max="13" width="12.453125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="18.26953125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.26953125" customWidth="1"/>
-    <col min="16" max="16" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.1796875" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="11.7265625" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="0" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:20">
       <c r="A1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:18">
+    <row r="2" spans="1:20">
+      <c r="M2" t="s">
+        <v>96</v>
+      </c>
+      <c r="S2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" s="17"/>
       <c r="B3" s="18" t="s">
         <v>33</v>
@@ -1401,8 +1430,14 @@
       <c r="R3" s="20" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:18">
+      <c r="S3" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="T3" s="19" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" s="23" t="s">
         <v>43</v>
       </c>
@@ -1439,11 +1474,14 @@
       <c r="L4" s="26">
         <v>10</v>
       </c>
+      <c r="M4" s="27"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="26"/>
       <c r="P4" s="25"/>
       <c r="Q4" s="25"/>
       <c r="R4" s="26"/>
     </row>
-    <row r="5" spans="1:18">
+    <row r="5" spans="1:20">
       <c r="A5" s="15" t="s">
         <v>44</v>
       </c>
@@ -1481,9 +1519,11 @@
         <v>10</v>
       </c>
       <c r="M5" s="11"/>
+      <c r="N5" s="33"/>
+      <c r="O5" s="12"/>
       <c r="R5" s="12"/>
     </row>
-    <row r="6" spans="1:18">
+    <row r="6" spans="1:20">
       <c r="A6" s="15" t="s">
         <v>45</v>
       </c>
@@ -1521,9 +1561,11 @@
         <v>10</v>
       </c>
       <c r="M6" s="11"/>
+      <c r="N6" s="33"/>
+      <c r="O6" s="12"/>
       <c r="R6" s="12"/>
     </row>
-    <row r="7" spans="1:18">
+    <row r="7" spans="1:20">
       <c r="A7" s="15" t="s">
         <v>46</v>
       </c>
@@ -1561,9 +1603,11 @@
         <v>10</v>
       </c>
       <c r="M7" s="11"/>
+      <c r="N7" s="33"/>
+      <c r="O7" s="12"/>
       <c r="R7" s="12"/>
     </row>
-    <row r="8" spans="1:18">
+    <row r="8" spans="1:20">
       <c r="A8" s="16" t="s">
         <v>47</v>
       </c>
@@ -1602,12 +1646,12 @@
       </c>
       <c r="M8" s="13"/>
       <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
+      <c r="O8" s="14"/>
       <c r="P8" s="3"/>
       <c r="Q8" s="3"/>
       <c r="R8" s="14"/>
     </row>
-    <row r="9" spans="1:18">
+    <row r="9" spans="1:20">
       <c r="A9" s="15" t="s">
         <v>48</v>
       </c>
@@ -1645,9 +1689,11 @@
         <v>10</v>
       </c>
       <c r="M9" s="11"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="12"/>
       <c r="R9" s="12"/>
     </row>
-    <row r="10" spans="1:18">
+    <row r="10" spans="1:20">
       <c r="A10" s="15" t="s">
         <v>49</v>
       </c>
@@ -1685,9 +1731,11 @@
         <v>10</v>
       </c>
       <c r="M10" s="11"/>
+      <c r="N10" s="33"/>
+      <c r="O10" s="12"/>
       <c r="R10" s="12"/>
     </row>
-    <row r="11" spans="1:18">
+    <row r="11" spans="1:20">
       <c r="A11" s="15" t="s">
         <v>50</v>
       </c>
@@ -1725,9 +1773,11 @@
         <v>10</v>
       </c>
       <c r="M11" s="11"/>
+      <c r="N11" s="33"/>
+      <c r="O11" s="12"/>
       <c r="R11" s="12"/>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:20">
       <c r="A12" s="15" t="s">
         <v>51</v>
       </c>
@@ -1765,9 +1815,11 @@
         <v>10</v>
       </c>
       <c r="M12" s="11"/>
+      <c r="N12" s="33"/>
+      <c r="O12" s="12"/>
       <c r="R12" s="12"/>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:20">
       <c r="A13" s="15" t="s">
         <v>52</v>
       </c>
@@ -1806,12 +1858,12 @@
       </c>
       <c r="M13" s="13"/>
       <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
+      <c r="O13" s="14"/>
       <c r="P13" s="3"/>
       <c r="Q13" s="3"/>
       <c r="R13" s="14"/>
     </row>
-    <row r="14" spans="1:18">
+    <row r="14" spans="1:20">
       <c r="A14" s="27" t="s">
         <v>67</v>
       </c>
@@ -1850,12 +1902,12 @@
       </c>
       <c r="M14" s="27"/>
       <c r="N14" s="25"/>
-      <c r="O14" s="25"/>
+      <c r="O14" s="26"/>
       <c r="P14" s="25"/>
       <c r="Q14" s="25"/>
       <c r="R14" s="26"/>
     </row>
-    <row r="15" spans="1:18">
+    <row r="15" spans="1:20">
       <c r="A15" s="11" t="s">
         <v>68</v>
       </c>
@@ -1893,9 +1945,11 @@
         <v>10</v>
       </c>
       <c r="M15" s="11"/>
+      <c r="N15" s="33"/>
+      <c r="O15" s="12"/>
       <c r="R15" s="12"/>
     </row>
-    <row r="16" spans="1:18">
+    <row r="16" spans="1:20">
       <c r="A16" s="11" t="s">
         <v>69</v>
       </c>
@@ -1933,9 +1987,11 @@
         <v>10</v>
       </c>
       <c r="M16" s="11"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="12"/>
       <c r="R16" s="12"/>
     </row>
-    <row r="17" spans="1:18">
+    <row r="17" spans="1:20">
       <c r="A17" s="11" t="s">
         <v>70</v>
       </c>
@@ -1973,9 +2029,11 @@
         <v>10</v>
       </c>
       <c r="M17" s="11"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="12"/>
       <c r="R17" s="12"/>
     </row>
-    <row r="18" spans="1:18">
+    <row r="18" spans="1:20">
       <c r="A18" s="13" t="s">
         <v>71</v>
       </c>
@@ -2014,12 +2072,12 @@
       </c>
       <c r="M18" s="13"/>
       <c r="N18" s="3"/>
-      <c r="O18" s="3"/>
+      <c r="O18" s="14"/>
       <c r="P18" s="3"/>
       <c r="Q18" s="3"/>
       <c r="R18" s="14"/>
     </row>
-    <row r="19" spans="1:18">
+    <row r="19" spans="1:20">
       <c r="A19" s="23" t="s">
         <v>73</v>
       </c>
@@ -2062,12 +2120,18 @@
       <c r="N19" s="25">
         <v>985.05200000000002</v>
       </c>
-      <c r="O19" s="25"/>
+      <c r="O19" s="26"/>
       <c r="P19" s="25"/>
       <c r="Q19" s="25"/>
       <c r="R19" s="26"/>
-    </row>
-    <row r="20" spans="1:18">
+      <c r="S19">
+        <v>1157.04</v>
+      </c>
+      <c r="T19">
+        <v>336.18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20" s="15" t="s">
         <v>74</v>
       </c>
@@ -2110,12 +2174,18 @@
       <c r="N20" s="33">
         <v>1455.43</v>
       </c>
-      <c r="O20" s="33" t="s">
+      <c r="O20" s="12" t="s">
         <v>92</v>
       </c>
       <c r="R20" s="12"/>
-    </row>
-    <row r="21" spans="1:18">
+      <c r="S20">
+        <v>1075.02</v>
+      </c>
+      <c r="T20">
+        <v>1063.1199999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
       <c r="A21" s="15" t="s">
         <v>75</v>
       </c>
@@ -2152,18 +2222,18 @@
       <c r="L21" s="12">
         <v>10</v>
       </c>
-      <c r="M21" s="33">
+      <c r="M21" s="11">
         <v>1094.49</v>
       </c>
       <c r="N21" s="33">
         <v>2801.37</v>
       </c>
-      <c r="O21" s="33" t="s">
+      <c r="O21" s="12" t="s">
         <v>92</v>
       </c>
       <c r="R21" s="12"/>
     </row>
-    <row r="22" spans="1:18">
+    <row r="22" spans="1:20">
       <c r="A22" s="15" t="s">
         <v>76</v>
       </c>
@@ -2206,12 +2276,12 @@
       <c r="N22" s="33">
         <v>4577.79</v>
       </c>
-      <c r="O22" s="33" t="s">
+      <c r="O22" s="12" t="s">
         <v>92</v>
       </c>
       <c r="R22" s="12"/>
     </row>
-    <row r="23" spans="1:18">
+    <row r="23" spans="1:20">
       <c r="A23" s="16" t="s">
         <v>77</v>
       </c>
@@ -2254,12 +2324,12 @@
       <c r="N23" s="3">
         <v>800.68499999999995</v>
       </c>
-      <c r="O23" s="3"/>
+      <c r="O23" s="14"/>
       <c r="P23" s="3"/>
       <c r="Q23" s="3"/>
       <c r="R23" s="14"/>
     </row>
-    <row r="24" spans="1:18">
+    <row r="24" spans="1:20">
       <c r="A24" s="15" t="s">
         <v>78</v>
       </c>
@@ -2293,7 +2363,7 @@
       <c r="K24">
         <v>10</v>
       </c>
-      <c r="L24" s="32">
+      <c r="L24">
         <v>10</v>
       </c>
       <c r="M24" s="27">
@@ -2302,12 +2372,18 @@
       <c r="N24" s="33">
         <v>513.24800000000005</v>
       </c>
-      <c r="O24" s="33" t="s">
+      <c r="O24" s="12" t="s">
         <v>93</v>
       </c>
       <c r="R24" s="12"/>
-    </row>
-    <row r="25" spans="1:18">
+      <c r="S24">
+        <v>953.72</v>
+      </c>
+      <c r="T24">
+        <v>276.27999999999997</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
       <c r="A25" s="15" t="s">
         <v>79</v>
       </c>
@@ -2350,12 +2426,12 @@
       <c r="N25" s="33">
         <v>8412.07</v>
       </c>
-      <c r="O25" s="33" t="s">
+      <c r="O25" s="12" t="s">
         <v>94</v>
       </c>
       <c r="R25" s="12"/>
     </row>
-    <row r="26" spans="1:18">
+    <row r="26" spans="1:20">
       <c r="A26" s="15" t="s">
         <v>80</v>
       </c>
@@ -2393,9 +2469,11 @@
         <v>10</v>
       </c>
       <c r="M26" s="11"/>
+      <c r="N26" s="33"/>
+      <c r="O26" s="12"/>
       <c r="R26" s="12"/>
     </row>
-    <row r="27" spans="1:18">
+    <row r="27" spans="1:20">
       <c r="A27" s="15" t="s">
         <v>81</v>
       </c>
@@ -2438,12 +2516,12 @@
       <c r="N27" s="33">
         <v>8412.59</v>
       </c>
-      <c r="O27" s="33" t="s">
+      <c r="O27" s="12" t="s">
         <v>94</v>
       </c>
       <c r="R27" s="12"/>
     </row>
-    <row r="28" spans="1:18">
+    <row r="28" spans="1:20">
       <c r="A28" s="15" t="s">
         <v>82</v>
       </c>
@@ -2486,14 +2564,14 @@
       <c r="N28" s="3">
         <v>2470.12</v>
       </c>
-      <c r="O28" s="33" t="s">
+      <c r="O28" s="12" t="s">
         <v>93</v>
       </c>
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="14"/>
     </row>
-    <row r="29" spans="1:18">
+    <row r="29" spans="1:20">
       <c r="A29" s="27" t="s">
         <v>83</v>
       </c>
@@ -2532,12 +2610,12 @@
       </c>
       <c r="M29" s="27"/>
       <c r="N29" s="25"/>
-      <c r="O29" s="25"/>
+      <c r="O29" s="26"/>
       <c r="P29" s="25"/>
       <c r="Q29" s="25"/>
       <c r="R29" s="26"/>
     </row>
-    <row r="30" spans="1:18">
+    <row r="30" spans="1:20">
       <c r="A30" s="11" t="s">
         <v>84</v>
       </c>
@@ -2575,9 +2653,11 @@
         <v>10</v>
       </c>
       <c r="M30" s="11"/>
+      <c r="N30" s="33"/>
+      <c r="O30" s="12"/>
       <c r="R30" s="12"/>
     </row>
-    <row r="31" spans="1:18">
+    <row r="31" spans="1:20">
       <c r="A31" s="11" t="s">
         <v>85</v>
       </c>
@@ -2615,9 +2695,11 @@
         <v>10</v>
       </c>
       <c r="M31" s="11"/>
+      <c r="N31" s="33"/>
+      <c r="O31" s="12"/>
       <c r="R31" s="12"/>
     </row>
-    <row r="32" spans="1:18">
+    <row r="32" spans="1:20">
       <c r="A32" s="11" t="s">
         <v>86</v>
       </c>
@@ -2655,6 +2737,8 @@
         <v>10</v>
       </c>
       <c r="M32" s="11"/>
+      <c r="N32" s="33"/>
+      <c r="O32" s="12"/>
       <c r="R32" s="12"/>
     </row>
     <row r="33" spans="1:18">
@@ -2696,7 +2780,7 @@
       </c>
       <c r="M33" s="13"/>
       <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
+      <c r="O33" s="14"/>
       <c r="P33" s="3"/>
       <c r="Q33" s="3"/>
       <c r="R33" s="14"/>

</xml_diff>